<commit_message>
with hourly time windows
</commit_message>
<xml_diff>
--- a/Practical/time_window_test.xlsx
+++ b/Practical/time_window_test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t>Demand</t>
   </si>
@@ -25,6 +25,9 @@
     <t>SERVICE TIME</t>
   </si>
   <si>
+    <t>delivery time</t>
+  </si>
+  <si>
     <t>ai</t>
   </si>
   <si>
@@ -67,6 +70,24 @@
     <t>DepotEnd</t>
   </si>
   <si>
+    <t>17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>13:00 - 13:30</t>
+  </si>
+  <si>
+    <t>12:00 - 13:00</t>
+  </si>
+  <si>
+    <t>14:00 - 14:30</t>
+  </si>
+  <si>
+    <t>13:00 - 14:00</t>
+  </si>
+  <si>
+    <t>11:00 - 11:30</t>
+  </si>
+  <si>
     <t>Vehicle</t>
   </si>
   <si>
@@ -74,6 +95,24 @@
   </si>
   <si>
     <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>V7</t>
+  </si>
+  <si>
+    <t>V8</t>
   </si>
 </sst>
 </file>
@@ -431,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,10 +489,13 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -461,186 +503,216 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>472</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>32400</v>
+      </c>
+      <c r="F3">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>426</v>
-      </c>
-      <c r="D3">
-        <v>693</v>
-      </c>
-      <c r="E3">
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>372</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>18000</v>
+      </c>
+      <c r="F4">
+        <v>19800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>428</v>
-      </c>
-      <c r="D4">
-        <v>486</v>
-      </c>
-      <c r="E4">
-        <v>2635</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
       <c r="C5">
-        <v>385</v>
-      </c>
-      <c r="D5">
-        <v>615</v>
+        <v>479</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
       </c>
       <c r="E5">
-        <v>2262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>14400</v>
+      </c>
+      <c r="F5">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
       <c r="C6">
-        <v>384</v>
-      </c>
-      <c r="D6">
-        <v>459</v>
+        <v>463</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>2437</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>32400</v>
+      </c>
+      <c r="F6">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7">
-        <v>434</v>
-      </c>
-      <c r="D7">
-        <v>684</v>
+        <v>406</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
       </c>
       <c r="E7">
-        <v>2071</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>32400</v>
+      </c>
+      <c r="F7">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>432</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>21600</v>
+      </c>
+      <c r="F8">
+        <v>23400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>446</v>
-      </c>
-      <c r="D8">
-        <v>570</v>
-      </c>
-      <c r="E8">
-        <v>2591</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
+      <c r="C9">
+        <v>455</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>18000</v>
+      </c>
+      <c r="F9">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>429</v>
       </c>
-      <c r="D9">
-        <v>632</v>
-      </c>
-      <c r="E9">
-        <v>2036</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>361</v>
-      </c>
-      <c r="D10">
-        <v>559</v>
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>2163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>14400</v>
+      </c>
+      <c r="F10">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>422</v>
-      </c>
-      <c r="D11">
-        <v>530</v>
+        <v>418</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>2576</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>18000</v>
+      </c>
+      <c r="F11">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>373</v>
-      </c>
-      <c r="D12">
-        <v>577</v>
+        <v>367</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
       </c>
       <c r="E12">
-        <v>2685</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>10800</v>
+      </c>
+      <c r="F12">
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -648,11 +720,11 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
       <c r="E13">
-        <v>5000</v>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>72000</v>
       </c>
     </row>
   </sheetData>
@@ -662,31 +734,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -704,78 +800,78 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F2">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H2">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="I2">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="J2">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="K2">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -783,450 +879,450 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>37</v>
+      </c>
+      <c r="H3">
+        <v>41</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
+      <c r="J3">
+        <v>25</v>
+      </c>
+      <c r="K3">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>16</v>
-      </c>
-      <c r="I3">
-        <v>15</v>
-      </c>
-      <c r="J3">
-        <v>14</v>
-      </c>
-      <c r="K3">
-        <v>9</v>
-      </c>
       <c r="L3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M3">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>29</v>
+      </c>
+      <c r="F4">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="G4">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>34</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>19</v>
-      </c>
-      <c r="H4">
-        <v>16</v>
-      </c>
-      <c r="I4">
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>13</v>
-      </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
       <c r="M4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>33</v>
+      </c>
+      <c r="H5">
+        <v>37</v>
+      </c>
+      <c r="I5">
+        <v>29</v>
+      </c>
+      <c r="J5">
+        <v>19</v>
+      </c>
+      <c r="K5">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>23</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>15</v>
-      </c>
-      <c r="I5">
-        <v>24</v>
-      </c>
-      <c r="J5">
-        <v>23</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
       <c r="L5">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M5">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>46</v>
+      </c>
+      <c r="J6">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>22</v>
+      </c>
+      <c r="L6">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>23</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>25</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <v>19</v>
-      </c>
-      <c r="L6">
-        <v>6</v>
-      </c>
       <c r="M6">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F7">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>62</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>24</v>
+      </c>
+      <c r="M7">
         <v>17</v>
-      </c>
-      <c r="I7">
-        <v>26</v>
-      </c>
-      <c r="J7">
-        <v>25</v>
-      </c>
-      <c r="K7">
-        <v>14</v>
-      </c>
-      <c r="L7">
-        <v>19</v>
-      </c>
-      <c r="M7">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F8">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G8">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="J8">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="K8">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="L8">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="M8">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E9">
+        <v>29</v>
+      </c>
+      <c r="F9">
+        <v>46</v>
+      </c>
+      <c r="G9">
+        <v>62</v>
+      </c>
+      <c r="H9">
+        <v>66</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>48</v>
+      </c>
+      <c r="K9">
         <v>24</v>
       </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>26</v>
-      </c>
-      <c r="H9">
-        <v>9</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>20</v>
-      </c>
       <c r="L9">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="M9">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>34</v>
+      </c>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10">
         <v>18</v>
       </c>
-      <c r="C10">
+      <c r="G10">
         <v>14</v>
       </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>23</v>
-      </c>
-      <c r="F10">
-        <v>6</v>
-      </c>
-      <c r="G10">
-        <v>25</v>
-      </c>
       <c r="H10">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L10">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="M10">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F11">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G11">
+        <v>38</v>
+      </c>
+      <c r="H11">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>24</v>
+      </c>
+      <c r="J11">
+        <v>24</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>14</v>
       </c>
-      <c r="H11">
-        <v>25</v>
-      </c>
-      <c r="I11">
-        <v>20</v>
-      </c>
-      <c r="J11">
-        <v>19</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>13</v>
-      </c>
       <c r="M11">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <v>28</v>
+      </c>
+      <c r="I12">
+        <v>38</v>
+      </c>
+      <c r="J12">
+        <v>26</v>
+      </c>
+      <c r="K12">
         <v>14</v>
       </c>
-      <c r="B12">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>17</v>
-      </c>
-      <c r="F12">
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <v>19</v>
-      </c>
-      <c r="H12">
-        <v>12</v>
-      </c>
-      <c r="I12">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>7</v>
-      </c>
-      <c r="J12">
-        <v>6</v>
-      </c>
-      <c r="K12">
-        <v>13</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
         <v>15</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>16</v>
-      </c>
       <c r="E13">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F13">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G13">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H13">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="I13">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="J13">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="K13">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L13">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1247,78 +1343,78 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>960</v>
+        <v>2400</v>
       </c>
       <c r="D2">
-        <v>963</v>
+        <v>1800</v>
       </c>
       <c r="E2">
-        <v>905</v>
+        <v>2640</v>
       </c>
       <c r="F2">
-        <v>1085</v>
+        <v>1080</v>
       </c>
       <c r="G2">
-        <v>663</v>
+        <v>2040</v>
       </c>
       <c r="H2">
-        <v>604</v>
+        <v>2760</v>
       </c>
       <c r="I2">
-        <v>1145</v>
+        <v>5400</v>
       </c>
       <c r="J2">
-        <v>1089</v>
+        <v>3240</v>
       </c>
       <c r="K2">
-        <v>1509</v>
+        <v>2520</v>
       </c>
       <c r="L2">
-        <v>725</v>
+        <v>840</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1326,450 +1422,450 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>966</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>482</v>
+        <v>1080</v>
       </c>
       <c r="E3">
-        <v>549</v>
+        <v>2400</v>
       </c>
       <c r="F3">
-        <v>849</v>
+        <v>2520</v>
       </c>
       <c r="G3">
-        <v>669</v>
+        <v>4440</v>
       </c>
       <c r="H3">
-        <v>963</v>
+        <v>4920</v>
       </c>
       <c r="I3">
-        <v>902</v>
+        <v>3000</v>
       </c>
       <c r="J3">
-        <v>840</v>
+        <v>3000</v>
       </c>
       <c r="K3">
-        <v>542</v>
+        <v>600</v>
       </c>
       <c r="L3">
-        <v>483</v>
+        <v>1560</v>
       </c>
       <c r="M3">
-        <v>961</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>968</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>482</v>
+        <v>1080</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1028</v>
+        <v>3480</v>
       </c>
       <c r="F4">
-        <v>360</v>
+        <v>1920</v>
       </c>
       <c r="G4">
-        <v>1143</v>
+        <v>3840</v>
       </c>
       <c r="H4">
-        <v>969</v>
+        <v>4320</v>
       </c>
       <c r="I4">
-        <v>542</v>
+        <v>3600</v>
       </c>
       <c r="J4">
-        <v>606</v>
+        <v>4080</v>
       </c>
       <c r="K4">
-        <v>780</v>
+        <v>1680</v>
       </c>
       <c r="L4">
-        <v>247</v>
+        <v>960</v>
       </c>
       <c r="M4">
-        <v>961</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>542</v>
+        <v>2400</v>
       </c>
       <c r="D5">
-        <v>1022</v>
+        <v>3480</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1384</v>
+        <v>2040</v>
       </c>
       <c r="G5">
-        <v>249</v>
+        <v>3960</v>
       </c>
       <c r="H5">
-        <v>907</v>
+        <v>4440</v>
       </c>
       <c r="I5">
-        <v>1445</v>
+        <v>3480</v>
       </c>
       <c r="J5">
-        <v>1382</v>
+        <v>2280</v>
       </c>
       <c r="K5">
-        <v>604</v>
+        <v>1800</v>
       </c>
       <c r="L5">
-        <v>1027</v>
+        <v>2520</v>
       </c>
       <c r="M5">
-        <v>908</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>1084</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>846</v>
+        <v>2520</v>
       </c>
       <c r="D6">
-        <v>362</v>
+        <v>1920</v>
       </c>
       <c r="E6">
-        <v>1386</v>
+        <v>2040</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1507</v>
+        <v>1920</v>
       </c>
       <c r="H6">
-        <v>727</v>
+        <v>2400</v>
       </c>
       <c r="I6">
-        <v>301</v>
+        <v>5520</v>
       </c>
       <c r="J6">
-        <v>363</v>
+        <v>2160</v>
       </c>
       <c r="K6">
-        <v>1149</v>
+        <v>2640</v>
       </c>
       <c r="L6">
-        <v>361</v>
+        <v>960</v>
       </c>
       <c r="M6">
-        <v>1085</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>663</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>667</v>
+        <v>4440</v>
       </c>
       <c r="D7">
-        <v>1143</v>
+        <v>3840</v>
       </c>
       <c r="E7">
-        <v>247</v>
+        <v>3960</v>
       </c>
       <c r="F7">
-        <v>1503</v>
+        <v>1920</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1026</v>
+        <v>720</v>
       </c>
       <c r="I7">
-        <v>1569</v>
+        <v>7440.000000000001</v>
       </c>
       <c r="J7">
-        <v>1505</v>
+        <v>1680</v>
       </c>
       <c r="K7">
-        <v>848</v>
+        <v>4560</v>
       </c>
       <c r="L7">
-        <v>1144</v>
+        <v>2880</v>
       </c>
       <c r="M7">
-        <v>667</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>963</v>
+        <v>4920</v>
       </c>
       <c r="D8">
-        <v>967</v>
+        <v>4320</v>
       </c>
       <c r="E8">
-        <v>909</v>
+        <v>4440</v>
       </c>
       <c r="F8">
-        <v>728</v>
+        <v>2400</v>
       </c>
       <c r="G8">
-        <v>1020</v>
+        <v>720</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>547</v>
+        <v>7920</v>
       </c>
       <c r="J8">
-        <v>481</v>
+        <v>2160</v>
       </c>
       <c r="K8">
-        <v>1503</v>
+        <v>5040</v>
       </c>
       <c r="L8">
-        <v>723</v>
+        <v>3360</v>
       </c>
       <c r="M8">
-        <v>606</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>1145</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="D9">
-        <v>547</v>
+        <v>3600</v>
       </c>
       <c r="E9">
-        <v>1448</v>
+        <v>3480</v>
       </c>
       <c r="F9">
-        <v>303</v>
+        <v>5520</v>
       </c>
       <c r="G9">
-        <v>1561</v>
+        <v>7440.000000000001</v>
       </c>
       <c r="H9">
-        <v>547</v>
+        <v>7920</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>60</v>
+        <v>5760</v>
       </c>
       <c r="K9">
-        <v>1207</v>
+        <v>2880</v>
       </c>
       <c r="L9">
-        <v>425</v>
+        <v>4560</v>
       </c>
       <c r="M9">
-        <v>1147</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>1081</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>840</v>
+        <v>3000</v>
       </c>
       <c r="D10">
-        <v>606</v>
+        <v>4080</v>
       </c>
       <c r="E10">
-        <v>1382</v>
+        <v>2280</v>
       </c>
       <c r="F10">
-        <v>366</v>
+        <v>2160</v>
       </c>
       <c r="G10">
-        <v>1500</v>
+        <v>1680</v>
       </c>
       <c r="H10">
-        <v>484</v>
+        <v>2160</v>
       </c>
       <c r="I10">
-        <v>62</v>
+        <v>5760</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1148</v>
+        <v>2880</v>
       </c>
       <c r="L10">
-        <v>361</v>
+        <v>3120</v>
       </c>
       <c r="M10">
-        <v>1080</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>1502</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>548</v>
+        <v>600</v>
       </c>
       <c r="D11">
-        <v>788</v>
+        <v>1680</v>
       </c>
       <c r="E11">
-        <v>601</v>
+        <v>1800</v>
       </c>
       <c r="F11">
-        <v>1148</v>
+        <v>2640</v>
       </c>
       <c r="G11">
-        <v>841</v>
+        <v>4560</v>
       </c>
       <c r="H11">
-        <v>1504</v>
+        <v>5040</v>
       </c>
       <c r="I11">
-        <v>1209</v>
+        <v>2880</v>
       </c>
       <c r="J11">
-        <v>1144</v>
+        <v>2880</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>784</v>
+        <v>1680</v>
       </c>
       <c r="M11">
-        <v>1504</v>
+        <v>2520</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>728</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>481</v>
+        <v>1560</v>
       </c>
       <c r="D12">
-        <v>245</v>
+        <v>960</v>
       </c>
       <c r="E12">
-        <v>1020</v>
+        <v>2520</v>
       </c>
       <c r="F12">
-        <v>368</v>
+        <v>960</v>
       </c>
       <c r="G12">
-        <v>1142</v>
+        <v>2880</v>
       </c>
       <c r="H12">
-        <v>726</v>
+        <v>3360</v>
       </c>
       <c r="I12">
-        <v>425</v>
+        <v>4560</v>
       </c>
       <c r="J12">
-        <v>366</v>
+        <v>3120</v>
       </c>
       <c r="K12">
-        <v>782</v>
+        <v>1680</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>721</v>
+        <v>840</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>961</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>968</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>902</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>1089</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>662</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>601</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1140</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>1086</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>1508</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>729</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>

</xml_diff>

<commit_message>
Working version - Reduced to 3 nodes for verification. Prints output route of optimal solution now. Constraints still to add: vehicle k cannot leave depotEnd (DepotEnd is end station). And later add ServiceTime
</commit_message>
<xml_diff>
--- a/Practical/time_window_test.xlsx
+++ b/Practical/time_window_test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>Demand</t>
   </si>
@@ -46,22 +46,16 @@
     <t>N3</t>
   </si>
   <si>
-    <t>N4</t>
-  </si>
-  <si>
     <t>DepotEnd</t>
   </si>
   <si>
-    <t>12:00 - 13:00</t>
-  </si>
-  <si>
-    <t>17:00 - 17:30</t>
-  </si>
-  <si>
-    <t>13:00 - 14:00</t>
-  </si>
-  <si>
-    <t>11:00 - 12:00</t>
+    <t>14:00 - 14:30</t>
+  </si>
+  <si>
+    <t>13:00 - 13:30</t>
+  </si>
+  <si>
+    <t>9:00 - 9:30</t>
   </si>
   <si>
     <t>Vehicle</t>
@@ -428,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>10800</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -473,19 +467,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>398</v>
+        <v>361</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>14400</v>
+        <v>21600</v>
       </c>
       <c r="F3">
-        <v>18000</v>
+        <v>23400</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -493,19 +487,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>409</v>
+        <v>440</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>32400</v>
+        <v>18000</v>
       </c>
       <c r="F4">
-        <v>34200</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -516,16 +510,16 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>18000</v>
+        <v>3600</v>
       </c>
       <c r="F5">
-        <v>21600</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -533,36 +527,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>398</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>10800</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>14400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>68400</v>
+        <v>46800</v>
       </c>
     </row>
   </sheetData>
@@ -580,17 +554,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -600,13 +574,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -622,11 +596,8 @@
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -634,133 +605,95 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="F2">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>36</v>
-      </c>
-      <c r="G3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F4">
-        <v>19</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>28</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>47</v>
-      </c>
-      <c r="G5">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>36</v>
-      </c>
-      <c r="D6">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>47</v>
-      </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>36</v>
-      </c>
-      <c r="F7">
-        <v>11</v>
-      </c>
-      <c r="G7">
         <v>0</v>
       </c>
     </row>
@@ -771,13 +704,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -793,11 +726,8 @@
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -805,22 +735,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3000</v>
+        <v>720</v>
       </c>
       <c r="D2">
-        <v>960</v>
+        <v>1560</v>
       </c>
       <c r="E2">
-        <v>4320</v>
+        <v>1320</v>
       </c>
       <c r="F2">
-        <v>1320</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -831,19 +758,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2040</v>
+        <v>2280</v>
       </c>
       <c r="E3">
-        <v>1320</v>
+        <v>600</v>
       </c>
       <c r="F3">
-        <v>4320</v>
-      </c>
-      <c r="G3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -851,22 +775,19 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>2040</v>
+        <v>2280</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>3360</v>
+        <v>1680</v>
       </c>
       <c r="F4">
-        <v>2280</v>
-      </c>
-      <c r="G4">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -874,22 +795,19 @@
         <v>0</v>
       </c>
       <c r="C5">
+        <v>600</v>
+      </c>
+      <c r="D5">
+        <v>1680</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>1320</v>
       </c>
-      <c r="D5">
-        <v>3360</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>5640</v>
-      </c>
-      <c r="G5">
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -897,41 +815,15 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>4320</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>2280</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>5640</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- added time window scaling to be able to use larger windows for testing - added constraints to implement actual depotstart and depotend functions - reduced the scope of the constraint "Vehicle leaves to next customer" to only normal nodes, not applicable to DepotEnd and DepotStart
</commit_message>
<xml_diff>
--- a/Practical/time_window_test.xlsx
+++ b/Practical/time_window_test.xlsx
@@ -49,13 +49,13 @@
     <t>DepotEnd</t>
   </si>
   <si>
-    <t>14:00 - 14:30</t>
-  </si>
-  <si>
-    <t>13:00 - 13:30</t>
-  </si>
-  <si>
-    <t>9:00 - 9:30</t>
+    <t>14:00 - 22:00</t>
+  </si>
+  <si>
+    <t>11:00 - 19:00</t>
+  </si>
+  <si>
+    <t>9:00 - 17:00</t>
   </si>
   <si>
     <t>Vehicle</t>
@@ -467,10 +467,10 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -479,7 +479,7 @@
         <v>21600</v>
       </c>
       <c r="F3">
-        <v>23400</v>
+        <v>50400</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -487,19 +487,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4">
-        <v>18000</v>
+        <v>10800</v>
       </c>
       <c r="F4">
-        <v>19800</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -507,10 +507,10 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>429</v>
+        <v>404</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -519,7 +519,7 @@
         <v>3600</v>
       </c>
       <c r="F5">
-        <v>5400</v>
+        <v>32400</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -536,7 +536,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>46800</v>
+        <v>100800</v>
       </c>
     </row>
   </sheetData>
@@ -605,13 +605,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -622,19 +622,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -642,19 +642,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F4">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -662,19 +662,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -685,13 +685,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D6">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -735,13 +735,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>720</v>
+        <v>3720</v>
       </c>
       <c r="D2">
-        <v>1560</v>
+        <v>6360</v>
       </c>
       <c r="E2">
-        <v>1320</v>
+        <v>1800</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -758,13 +758,13 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2280</v>
+        <v>2640</v>
       </c>
       <c r="E3">
-        <v>600</v>
+        <v>2400</v>
       </c>
       <c r="F3">
-        <v>720</v>
+        <v>3720</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -775,16 +775,16 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>2280</v>
+        <v>2640</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1680</v>
+        <v>5040</v>
       </c>
       <c r="F4">
-        <v>1560</v>
+        <v>6360</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -795,16 +795,16 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>600</v>
+        <v>2400</v>
       </c>
       <c r="D5">
-        <v>1680</v>
+        <v>5040</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1320</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="6" spans="1:6">

</xml_diff>

<commit_message>
it works - bless
</commit_message>
<xml_diff>
--- a/Practical/time_window_test.xlsx
+++ b/Practical/time_window_test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>Demand</t>
   </si>
@@ -46,16 +46,52 @@
     <t>N3</t>
   </si>
   <si>
+    <t>N4</t>
+  </si>
+  <si>
+    <t>N5</t>
+  </si>
+  <si>
+    <t>N6</t>
+  </si>
+  <si>
+    <t>N7</t>
+  </si>
+  <si>
+    <t>N8</t>
+  </si>
+  <si>
+    <t>N9</t>
+  </si>
+  <si>
+    <t>N10</t>
+  </si>
+  <si>
     <t>DepotEnd</t>
   </si>
   <si>
-    <t>14:00 - 22:00</t>
+    <t>15:00 - 23:00</t>
+  </si>
+  <si>
+    <t>16:00 - 24:00</t>
+  </si>
+  <si>
+    <t>9:00 - 17:00</t>
   </si>
   <si>
     <t>11:00 - 19:00</t>
   </si>
   <si>
-    <t>9:00 - 17:00</t>
+    <t>15:00 - 19:00</t>
+  </si>
+  <si>
+    <t>13:00 - 17:00</t>
+  </si>
+  <si>
+    <t>12:00 - 20:00</t>
+  </si>
+  <si>
+    <t>17:00 - 21:00</t>
   </si>
   <si>
     <t>Vehicle</t>
@@ -422,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,19 +503,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>375</v>
+        <v>417</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E3">
-        <v>21600</v>
+        <v>25200</v>
       </c>
       <c r="F3">
-        <v>50400</v>
+        <v>54000</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -487,19 +523,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E4">
-        <v>10800</v>
+        <v>28800</v>
       </c>
       <c r="F4">
-        <v>39600</v>
+        <v>57600</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -507,13 +543,13 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>404</v>
+        <v>460</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>3600</v>
@@ -527,16 +563,156 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>393</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
       </c>
       <c r="E6">
+        <v>10800</v>
+      </c>
+      <c r="F6">
+        <v>39600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>100800</v>
+      <c r="C7">
+        <v>429</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>25200</v>
+      </c>
+      <c r="F7">
+        <v>39600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>413</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>25200</v>
+      </c>
+      <c r="F8">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>401</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>18000</v>
+      </c>
+      <c r="F9">
+        <v>32400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>432</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <v>14400</v>
+      </c>
+      <c r="F10">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>364</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>32400</v>
+      </c>
+      <c r="F11">
+        <v>46800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>407</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>18000</v>
+      </c>
+      <c r="F12">
+        <v>32400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>115200</v>
       </c>
     </row>
   </sheetData>
@@ -554,17 +730,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -574,13 +750,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -596,8 +772,29 @@
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -605,95 +802,487 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D2">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
         <v>15</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>26</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>30</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>34</v>
+      </c>
+      <c r="H3">
         <v>31</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>22</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="I3">
+        <v>19</v>
+      </c>
+      <c r="J3">
+        <v>43</v>
+      </c>
+      <c r="K3">
+        <v>30</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="F4">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>32</v>
+      </c>
+      <c r="I4">
+        <v>26</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <v>40</v>
+      </c>
+      <c r="M4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D5">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>14</v>
+      </c>
+      <c r="K5">
+        <v>17</v>
+      </c>
+      <c r="L5">
+        <v>24</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <v>13</v>
+      </c>
+      <c r="J6">
+        <v>19</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
+      <c r="L6">
         <v>31</v>
       </c>
-      <c r="D6">
-        <v>53</v>
-      </c>
-      <c r="E6">
+      <c r="M6">
         <v>15</v>
       </c>
-      <c r="F6">
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>21</v>
+      </c>
+      <c r="K7">
+        <v>18</v>
+      </c>
+      <c r="L7">
+        <v>33</v>
+      </c>
+      <c r="M7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>18</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>42</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>24</v>
+      </c>
+      <c r="K9">
+        <v>17</v>
+      </c>
+      <c r="L9">
+        <v>24</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>19</v>
+      </c>
+      <c r="G10">
+        <v>21</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>29</v>
+      </c>
+      <c r="L10">
+        <v>38</v>
+      </c>
+      <c r="M10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>18</v>
+      </c>
+      <c r="H11">
+        <v>13</v>
+      </c>
+      <c r="I11">
+        <v>17</v>
+      </c>
+      <c r="J11">
+        <v>29</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>41</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>31</v>
+      </c>
+      <c r="G12">
+        <v>33</v>
+      </c>
+      <c r="H12">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>38</v>
+      </c>
+      <c r="K12">
+        <v>41</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>26</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>30</v>
+      </c>
+      <c r="M13">
         <v>0</v>
       </c>
     </row>
@@ -704,13 +1293,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -726,8 +1315,29 @@
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -735,19 +1345,40 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3720</v>
+        <v>2280</v>
       </c>
       <c r="D2">
-        <v>6360</v>
+        <v>3360</v>
       </c>
       <c r="E2">
+        <v>1440</v>
+      </c>
+      <c r="F2">
         <v>1800</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>2040</v>
+      </c>
+      <c r="H2">
+        <v>1440</v>
+      </c>
+      <c r="I2">
+        <v>720</v>
+      </c>
+      <c r="J2">
+        <v>3120</v>
+      </c>
+      <c r="K2">
+        <v>1320</v>
+      </c>
+      <c r="L2">
+        <v>3600</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -758,16 +1389,37 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2640</v>
+        <v>5400</v>
       </c>
       <c r="E3">
-        <v>2400</v>
+        <v>3480</v>
       </c>
       <c r="F3">
+        <v>3840</v>
+      </c>
+      <c r="G3">
+        <v>4080</v>
+      </c>
+      <c r="H3">
         <v>3720</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="I3">
+        <v>2280</v>
+      </c>
+      <c r="J3">
+        <v>5160</v>
+      </c>
+      <c r="K3">
+        <v>3600</v>
+      </c>
+      <c r="L3">
+        <v>1320</v>
+      </c>
+      <c r="M3">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -775,19 +1427,40 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>2640</v>
+        <v>5400</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>5040</v>
+        <v>1920</v>
       </c>
       <c r="F4">
-        <v>6360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>2520</v>
+      </c>
+      <c r="G4">
+        <v>2760</v>
+      </c>
+      <c r="H4">
+        <v>3840</v>
+      </c>
+      <c r="I4">
+        <v>3120</v>
+      </c>
+      <c r="J4">
+        <v>240</v>
+      </c>
+      <c r="K4">
+        <v>3720</v>
+      </c>
+      <c r="L4">
+        <v>4800</v>
+      </c>
+      <c r="M4">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -795,19 +1468,40 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>2400</v>
+        <v>3480</v>
       </c>
       <c r="D5">
-        <v>5040</v>
+        <v>1920</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>840</v>
+      </c>
+      <c r="G5">
+        <v>1080</v>
+      </c>
+      <c r="H5">
+        <v>2160</v>
+      </c>
+      <c r="I5">
+        <v>1200</v>
+      </c>
+      <c r="J5">
+        <v>1680</v>
+      </c>
+      <c r="K5">
+        <v>2040</v>
+      </c>
+      <c r="L5">
+        <v>2880</v>
+      </c>
+      <c r="M5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -815,15 +1509,323 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3840</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2520</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>240</v>
+      </c>
+      <c r="H6">
+        <v>1320</v>
+      </c>
+      <c r="I6">
+        <v>1560</v>
+      </c>
+      <c r="J6">
+        <v>2280</v>
+      </c>
+      <c r="K6">
+        <v>1920</v>
+      </c>
+      <c r="L6">
+        <v>3720</v>
+      </c>
+      <c r="M6">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>4080</v>
+      </c>
+      <c r="D7">
+        <v>2760</v>
+      </c>
+      <c r="E7">
+        <v>1080</v>
+      </c>
+      <c r="F7">
+        <v>240</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1080</v>
+      </c>
+      <c r="I7">
+        <v>1800</v>
+      </c>
+      <c r="J7">
+        <v>2520</v>
+      </c>
+      <c r="K7">
+        <v>2160</v>
+      </c>
+      <c r="L7">
+        <v>3960</v>
+      </c>
+      <c r="M7">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>3720</v>
+      </c>
+      <c r="D8">
+        <v>3840</v>
+      </c>
+      <c r="E8">
+        <v>2160</v>
+      </c>
+      <c r="F8">
+        <v>1320</v>
+      </c>
+      <c r="G8">
+        <v>1080</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>2160</v>
+      </c>
+      <c r="J8">
+        <v>3600</v>
+      </c>
+      <c r="K8">
+        <v>1560</v>
+      </c>
+      <c r="L8">
+        <v>5040</v>
+      </c>
+      <c r="M8">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>2280</v>
+      </c>
+      <c r="D9">
+        <v>3120</v>
+      </c>
+      <c r="E9">
+        <v>1200</v>
+      </c>
+      <c r="F9">
+        <v>1560</v>
+      </c>
+      <c r="G9">
+        <v>1800</v>
+      </c>
+      <c r="H9">
+        <v>2160</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>2880</v>
+      </c>
+      <c r="K9">
+        <v>2040</v>
+      </c>
+      <c r="L9">
+        <v>2880</v>
+      </c>
+      <c r="M9">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>5160</v>
+      </c>
+      <c r="D10">
+        <v>240</v>
+      </c>
+      <c r="E10">
+        <v>1680</v>
+      </c>
+      <c r="F10">
+        <v>2280</v>
+      </c>
+      <c r="G10">
+        <v>2520</v>
+      </c>
+      <c r="H10">
+        <v>3600</v>
+      </c>
+      <c r="I10">
+        <v>2880</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>3480</v>
+      </c>
+      <c r="L10">
+        <v>4560</v>
+      </c>
+      <c r="M10">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>3600</v>
+      </c>
+      <c r="D11">
+        <v>3720</v>
+      </c>
+      <c r="E11">
+        <v>2040</v>
+      </c>
+      <c r="F11">
+        <v>1920</v>
+      </c>
+      <c r="G11">
+        <v>2160</v>
+      </c>
+      <c r="H11">
+        <v>1560</v>
+      </c>
+      <c r="I11">
+        <v>2040</v>
+      </c>
+      <c r="J11">
+        <v>3480</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>4920</v>
+      </c>
+      <c r="M11">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1320</v>
+      </c>
+      <c r="D12">
+        <v>4800</v>
+      </c>
+      <c r="E12">
+        <v>2880</v>
+      </c>
+      <c r="F12">
+        <v>3720</v>
+      </c>
+      <c r="G12">
+        <v>3960</v>
+      </c>
+      <c r="H12">
+        <v>5040</v>
+      </c>
+      <c r="I12">
+        <v>2880</v>
+      </c>
+      <c r="J12">
+        <v>4560</v>
+      </c>
+      <c r="K12">
+        <v>4920</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
it works - bless v2
</commit_message>
<xml_diff>
--- a/Practical/time_window_test.xlsx
+++ b/Practical/time_window_test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
   <si>
     <t>Demand</t>
   </si>
@@ -67,31 +67,52 @@
     <t>N10</t>
   </si>
   <si>
+    <t>N11</t>
+  </si>
+  <si>
+    <t>N12</t>
+  </si>
+  <si>
+    <t>N13</t>
+  </si>
+  <si>
+    <t>N14</t>
+  </si>
+  <si>
+    <t>N15</t>
+  </si>
+  <si>
     <t>DepotEnd</t>
   </si>
   <si>
-    <t>15:00 - 23:00</t>
+    <t>13:00 - 21:00</t>
   </si>
   <si>
     <t>16:00 - 24:00</t>
   </si>
   <si>
+    <t>11:00 - 15:00</t>
+  </si>
+  <si>
     <t>9:00 - 17:00</t>
   </si>
   <si>
-    <t>11:00 - 19:00</t>
-  </si>
-  <si>
-    <t>15:00 - 19:00</t>
+    <t>10:00 - 18:00</t>
+  </si>
+  <si>
+    <t>16:00 - 20:00</t>
+  </si>
+  <si>
+    <t>12:00 - 20:00</t>
   </si>
   <si>
     <t>13:00 - 17:00</t>
   </si>
   <si>
-    <t>12:00 - 20:00</t>
-  </si>
-  <si>
-    <t>17:00 - 21:00</t>
+    <t>10:00 - 14:00</t>
+  </si>
+  <si>
+    <t>9:00 - 13:00</t>
   </si>
   <si>
     <t>Vehicle</t>
@@ -458,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,19 +524,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>417</v>
+        <v>441</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E3">
-        <v>25200</v>
+        <v>18000</v>
       </c>
       <c r="F3">
-        <v>54000</v>
+        <v>46800</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -523,13 +544,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>28800</v>
@@ -543,19 +564,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>460</v>
+        <v>363</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E5">
-        <v>3600</v>
+        <v>10800</v>
       </c>
       <c r="F5">
-        <v>32400</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -563,19 +584,19 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6">
-        <v>10800</v>
+        <v>18000</v>
       </c>
       <c r="F6">
-        <v>39600</v>
+        <v>46800</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -583,19 +604,19 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>429</v>
+        <v>466</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E7">
-        <v>25200</v>
+        <v>3600</v>
       </c>
       <c r="F7">
-        <v>39600</v>
+        <v>32400</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -603,19 +624,19 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>413</v>
+        <v>437</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E8">
-        <v>25200</v>
+        <v>7200</v>
       </c>
       <c r="F8">
-        <v>54000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -623,19 +644,19 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>401</v>
+        <v>443</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E9">
-        <v>18000</v>
+        <v>28800</v>
       </c>
       <c r="F9">
-        <v>32400</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -646,10 +667,10 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>14400</v>
@@ -663,19 +684,19 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>364</v>
+        <v>409</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>32400</v>
+        <v>7200</v>
       </c>
       <c r="F11">
-        <v>46800</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -683,13 +704,13 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>407</v>
+        <v>448</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>18000</v>
@@ -703,15 +724,115 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>406</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
       </c>
       <c r="E13">
+        <v>18000</v>
+      </c>
+      <c r="F13">
+        <v>32400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>474</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>18000</v>
+      </c>
+      <c r="F14">
+        <v>46800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>398</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <v>7200</v>
+      </c>
+      <c r="F15">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>388</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16">
+        <v>3600</v>
+      </c>
+      <c r="F16">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>476</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>10800</v>
+      </c>
+      <c r="F17">
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="F18">
         <v>115200</v>
       </c>
     </row>
@@ -730,17 +851,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -750,13 +871,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:18">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -793,8 +914,23 @@
       <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -802,487 +938,947 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D2">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>35</v>
+      </c>
+      <c r="H2">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>39</v>
+      </c>
+      <c r="K2">
+        <v>46</v>
+      </c>
+      <c r="L2">
+        <v>25</v>
+      </c>
+      <c r="M2">
         <v>12</v>
       </c>
-      <c r="F2">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>17</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>26</v>
-      </c>
-      <c r="K2">
-        <v>11</v>
-      </c>
-      <c r="L2">
-        <v>30</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>41</v>
+      </c>
+      <c r="O2">
+        <v>51</v>
+      </c>
+      <c r="P2">
+        <v>35</v>
+      </c>
+      <c r="Q2">
+        <v>13</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
         <v>19</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="I3">
+        <v>28</v>
+      </c>
+      <c r="J3">
+        <v>41</v>
+      </c>
+      <c r="K3">
+        <v>14</v>
+      </c>
+      <c r="L3">
         <v>45</v>
       </c>
-      <c r="E3">
+      <c r="M3">
+        <v>26</v>
+      </c>
+      <c r="N3">
+        <v>23</v>
+      </c>
+      <c r="O3">
         <v>29</v>
       </c>
-      <c r="F3">
-        <v>32</v>
-      </c>
-      <c r="G3">
-        <v>34</v>
-      </c>
-      <c r="H3">
-        <v>31</v>
-      </c>
-      <c r="I3">
-        <v>19</v>
-      </c>
-      <c r="J3">
-        <v>43</v>
-      </c>
-      <c r="K3">
-        <v>30</v>
-      </c>
-      <c r="L3">
-        <v>11</v>
-      </c>
-      <c r="M3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="P3">
+        <v>13</v>
+      </c>
+      <c r="Q3">
+        <v>39</v>
+      </c>
+      <c r="R3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H4">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>35</v>
+      </c>
+      <c r="J4">
+        <v>36</v>
+      </c>
+      <c r="K4">
+        <v>43</v>
+      </c>
+      <c r="L4">
+        <v>22</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>36</v>
+      </c>
+      <c r="O4">
+        <v>48</v>
+      </c>
+      <c r="P4">
         <v>32</v>
       </c>
-      <c r="I4">
-        <v>26</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>31</v>
-      </c>
-      <c r="L4">
-        <v>40</v>
-      </c>
-      <c r="M4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>14</v>
+      </c>
+      <c r="I5">
         <v>29</v>
       </c>
-      <c r="D5">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="J5">
+        <v>36</v>
+      </c>
+      <c r="K5">
+        <v>43</v>
+      </c>
+      <c r="L5">
+        <v>22</v>
+      </c>
+      <c r="M5">
         <v>7</v>
       </c>
-      <c r="G5">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>18</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5">
-        <v>14</v>
-      </c>
-      <c r="K5">
-        <v>17</v>
-      </c>
-      <c r="L5">
-        <v>24</v>
-      </c>
-      <c r="M5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>48</v>
+      </c>
+      <c r="P5">
+        <v>32</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="H6">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I6">
+        <v>35</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>23</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6">
         <v>13</v>
       </c>
-      <c r="J6">
-        <v>19</v>
-      </c>
-      <c r="K6">
-        <v>16</v>
-      </c>
-      <c r="L6">
-        <v>31</v>
-      </c>
-      <c r="M6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <v>36</v>
+      </c>
+      <c r="O6">
+        <v>28</v>
+      </c>
+      <c r="P6">
+        <v>20</v>
+      </c>
+      <c r="Q6">
+        <v>26</v>
+      </c>
+      <c r="R6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C7">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I7">
         <v>15</v>
       </c>
       <c r="J7">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="K7">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L7">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="M7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <v>28</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="Q7">
+        <v>26</v>
+      </c>
+      <c r="R7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>18</v>
+      </c>
+      <c r="G8">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>31</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>17</v>
+      </c>
+      <c r="J8">
+        <v>26</v>
+      </c>
+      <c r="K8">
+        <v>29</v>
+      </c>
+      <c r="L8">
+        <v>30</v>
+      </c>
+      <c r="M8">
+        <v>11</v>
+      </c>
+      <c r="N8">
         <v>18</v>
       </c>
-      <c r="F8">
-        <v>11</v>
-      </c>
-      <c r="G8">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
+      <c r="O8">
+        <v>34</v>
+      </c>
+      <c r="P8">
         <v>18</v>
       </c>
-      <c r="J8">
-        <v>30</v>
-      </c>
-      <c r="K8">
-        <v>13</v>
-      </c>
-      <c r="L8">
-        <v>42</v>
-      </c>
-      <c r="M8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="Q8">
+        <v>20</v>
+      </c>
+      <c r="R8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C9">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F9">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="G9">
         <v>15</v>
       </c>
       <c r="H9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="K9">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="L9">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="M9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>28</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <v>43</v>
+      </c>
+      <c r="P9">
+        <v>27</v>
+      </c>
+      <c r="Q9">
+        <v>27</v>
+      </c>
+      <c r="R9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10">
+        <v>39</v>
+      </c>
+      <c r="C10">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>38</v>
+      </c>
+      <c r="H10">
         <v>26</v>
       </c>
-      <c r="C10">
+      <c r="I10">
         <v>43</v>
       </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>27</v>
+      </c>
+      <c r="L10">
         <v>14</v>
       </c>
-      <c r="F10">
-        <v>19</v>
-      </c>
-      <c r="G10">
-        <v>21</v>
-      </c>
-      <c r="H10">
-        <v>30</v>
-      </c>
-      <c r="I10">
-        <v>24</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
+      <c r="M10">
         <v>29</v>
       </c>
-      <c r="L10">
-        <v>38</v>
-      </c>
-      <c r="M10">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>44</v>
+      </c>
+      <c r="O10">
+        <v>12</v>
+      </c>
+      <c r="P10">
+        <v>28</v>
+      </c>
+      <c r="Q10">
+        <v>42</v>
+      </c>
+      <c r="R10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>43</v>
+      </c>
+      <c r="E11">
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>29</v>
+      </c>
+      <c r="I11">
+        <v>38</v>
+      </c>
+      <c r="J11">
+        <v>27</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>31</v>
+      </c>
+      <c r="M11">
+        <v>36</v>
+      </c>
+      <c r="N11">
+        <v>33</v>
+      </c>
+      <c r="O11">
+        <v>15</v>
+      </c>
+      <c r="P11">
         <v>11</v>
       </c>
-      <c r="C11">
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <v>31</v>
-      </c>
-      <c r="E11">
-        <v>17</v>
-      </c>
-      <c r="F11">
-        <v>16</v>
-      </c>
-      <c r="G11">
-        <v>18</v>
-      </c>
-      <c r="H11">
-        <v>13</v>
-      </c>
-      <c r="I11">
-        <v>17</v>
-      </c>
-      <c r="J11">
-        <v>29</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>41</v>
-      </c>
-      <c r="M11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="Q11">
+        <v>49</v>
+      </c>
+      <c r="R11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>42</v>
+      </c>
+      <c r="H12">
         <v>30</v>
       </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>40</v>
-      </c>
-      <c r="E12">
-        <v>24</v>
-      </c>
-      <c r="F12">
+      <c r="I12">
+        <v>47</v>
+      </c>
+      <c r="J12">
+        <v>14</v>
+      </c>
+      <c r="K12">
         <v>31</v>
       </c>
-      <c r="G12">
-        <v>33</v>
-      </c>
-      <c r="H12">
-        <v>42</v>
-      </c>
-      <c r="I12">
-        <v>24</v>
-      </c>
-      <c r="J12">
-        <v>38</v>
-      </c>
-      <c r="K12">
-        <v>41</v>
-      </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>19</v>
+      </c>
+      <c r="N12">
+        <v>48</v>
+      </c>
+      <c r="O12">
+        <v>26</v>
+      </c>
+      <c r="P12">
+        <v>32</v>
+      </c>
+      <c r="Q12">
+        <v>28</v>
+      </c>
+      <c r="R12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C13">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>28</v>
+      </c>
+      <c r="J13">
+        <v>29</v>
+      </c>
+      <c r="K13">
+        <v>36</v>
+      </c>
+      <c r="L13">
         <v>19</v>
       </c>
-      <c r="D13">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>29</v>
+      </c>
+      <c r="O13">
+        <v>41</v>
+      </c>
+      <c r="P13">
+        <v>25</v>
+      </c>
+      <c r="Q13">
+        <v>13</v>
+      </c>
+      <c r="R13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>18</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>44</v>
+      </c>
+      <c r="K14">
+        <v>33</v>
+      </c>
+      <c r="L14">
+        <v>48</v>
+      </c>
+      <c r="M14">
+        <v>29</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>38</v>
+      </c>
+      <c r="P14">
+        <v>22</v>
+      </c>
+      <c r="Q14">
         <v>28</v>
       </c>
-      <c r="E13">
+      <c r="R14">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>48</v>
+      </c>
+      <c r="E15">
+        <v>48</v>
+      </c>
+      <c r="F15">
+        <v>28</v>
+      </c>
+      <c r="G15">
+        <v>28</v>
+      </c>
+      <c r="H15">
+        <v>34</v>
+      </c>
+      <c r="I15">
+        <v>43</v>
+      </c>
+      <c r="J15">
         <v>12</v>
       </c>
-      <c r="F13">
+      <c r="K15">
         <v>15</v>
       </c>
-      <c r="G13">
-        <v>17</v>
-      </c>
-      <c r="H13">
+      <c r="L15">
+        <v>26</v>
+      </c>
+      <c r="M15">
+        <v>41</v>
+      </c>
+      <c r="N15">
+        <v>38</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>16</v>
+      </c>
+      <c r="Q15">
+        <v>54</v>
+      </c>
+      <c r="R15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
         <v>12</v>
       </c>
-      <c r="I13">
+      <c r="H16">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <v>27</v>
+      </c>
+      <c r="J16">
+        <v>28</v>
+      </c>
+      <c r="K16">
+        <v>11</v>
+      </c>
+      <c r="L16">
+        <v>32</v>
+      </c>
+      <c r="M16">
+        <v>25</v>
+      </c>
+      <c r="N16">
+        <v>22</v>
+      </c>
+      <c r="O16">
+        <v>16</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>38</v>
+      </c>
+      <c r="R16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>39</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
         <v>6</v>
       </c>
-      <c r="J13">
+      <c r="F17">
         <v>26</v>
       </c>
-      <c r="K13">
+      <c r="G17">
+        <v>26</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <v>27</v>
+      </c>
+      <c r="J17">
+        <v>42</v>
+      </c>
+      <c r="K17">
+        <v>49</v>
+      </c>
+      <c r="L17">
+        <v>28</v>
+      </c>
+      <c r="M17">
+        <v>13</v>
+      </c>
+      <c r="N17">
+        <v>28</v>
+      </c>
+      <c r="O17">
+        <v>54</v>
+      </c>
+      <c r="P17">
+        <v>38</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
         <v>11</v>
       </c>
-      <c r="L13">
-        <v>30</v>
-      </c>
-      <c r="M13">
+      <c r="F18">
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <v>35</v>
+      </c>
+      <c r="H18">
+        <v>23</v>
+      </c>
+      <c r="I18">
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <v>39</v>
+      </c>
+      <c r="K18">
+        <v>46</v>
+      </c>
+      <c r="L18">
+        <v>25</v>
+      </c>
+      <c r="M18">
+        <v>12</v>
+      </c>
+      <c r="N18">
+        <v>41</v>
+      </c>
+      <c r="O18">
+        <v>51</v>
+      </c>
+      <c r="P18">
+        <v>35</v>
+      </c>
+      <c r="Q18">
+        <v>13</v>
+      </c>
+      <c r="R18">
         <v>0</v>
       </c>
     </row>
@@ -1293,13 +1889,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:18">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1336,8 +1932,23 @@
       <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1345,40 +1956,55 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2280</v>
+        <v>4560</v>
       </c>
       <c r="D2">
-        <v>3360</v>
+        <v>600</v>
       </c>
       <c r="E2">
+        <v>1320</v>
+      </c>
+      <c r="F2">
+        <v>2760</v>
+      </c>
+      <c r="G2">
+        <v>4200</v>
+      </c>
+      <c r="H2">
+        <v>2760</v>
+      </c>
+      <c r="I2">
+        <v>4800</v>
+      </c>
+      <c r="J2">
+        <v>4680</v>
+      </c>
+      <c r="K2">
+        <v>5520</v>
+      </c>
+      <c r="L2">
+        <v>3000</v>
+      </c>
+      <c r="M2">
         <v>1440</v>
       </c>
-      <c r="F2">
-        <v>1800</v>
-      </c>
-      <c r="G2">
-        <v>2040</v>
-      </c>
-      <c r="H2">
-        <v>1440</v>
-      </c>
-      <c r="I2">
-        <v>720</v>
-      </c>
-      <c r="J2">
-        <v>3120</v>
-      </c>
-      <c r="K2">
-        <v>1320</v>
-      </c>
-      <c r="L2">
-        <v>3600</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>4920</v>
+      </c>
+      <c r="O2">
+        <v>6120</v>
+      </c>
+      <c r="P2">
+        <v>4200</v>
+      </c>
+      <c r="Q2">
+        <v>1560</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1389,37 +2015,52 @@
         <v>0</v>
       </c>
       <c r="D3">
+        <v>3960</v>
+      </c>
+      <c r="E3">
+        <v>3960</v>
+      </c>
+      <c r="F3">
+        <v>3960</v>
+      </c>
+      <c r="G3">
+        <v>1560</v>
+      </c>
+      <c r="H3">
+        <v>2280</v>
+      </c>
+      <c r="I3">
+        <v>3360</v>
+      </c>
+      <c r="J3">
+        <v>4920</v>
+      </c>
+      <c r="K3">
+        <v>1680</v>
+      </c>
+      <c r="L3">
         <v>5400</v>
       </c>
-      <c r="E3">
+      <c r="M3">
+        <v>3120</v>
+      </c>
+      <c r="N3">
+        <v>2760</v>
+      </c>
+      <c r="O3">
         <v>3480</v>
       </c>
-      <c r="F3">
-        <v>3840</v>
-      </c>
-      <c r="G3">
-        <v>4080</v>
-      </c>
-      <c r="H3">
-        <v>3720</v>
-      </c>
-      <c r="I3">
-        <v>2280</v>
-      </c>
-      <c r="J3">
-        <v>5160</v>
-      </c>
-      <c r="K3">
-        <v>3600</v>
-      </c>
-      <c r="L3">
-        <v>1320</v>
-      </c>
-      <c r="M3">
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="P3">
+        <v>1560</v>
+      </c>
+      <c r="Q3">
+        <v>4680</v>
+      </c>
+      <c r="R3">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1427,40 +2068,55 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5400</v>
+        <v>3960</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1920</v>
+        <v>720</v>
       </c>
       <c r="F4">
-        <v>2520</v>
+        <v>2400</v>
       </c>
       <c r="G4">
-        <v>2760</v>
+        <v>3600</v>
       </c>
       <c r="H4">
+        <v>2160</v>
+      </c>
+      <c r="I4">
+        <v>4200</v>
+      </c>
+      <c r="J4">
+        <v>4320</v>
+      </c>
+      <c r="K4">
+        <v>5160</v>
+      </c>
+      <c r="L4">
+        <v>2640</v>
+      </c>
+      <c r="M4">
+        <v>840</v>
+      </c>
+      <c r="N4">
+        <v>4320</v>
+      </c>
+      <c r="O4">
+        <v>5760</v>
+      </c>
+      <c r="P4">
         <v>3840</v>
       </c>
-      <c r="I4">
-        <v>3120</v>
-      </c>
-      <c r="J4">
-        <v>240</v>
-      </c>
-      <c r="K4">
-        <v>3720</v>
-      </c>
-      <c r="L4">
-        <v>4800</v>
-      </c>
-      <c r="M4">
-        <v>3360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="Q4">
+        <v>960</v>
+      </c>
+      <c r="R4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1468,40 +2124,55 @@
         <v>0</v>
       </c>
       <c r="C5">
+        <v>3960</v>
+      </c>
+      <c r="D5">
+        <v>720</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2400</v>
+      </c>
+      <c r="G5">
+        <v>2880</v>
+      </c>
+      <c r="H5">
+        <v>1680</v>
+      </c>
+      <c r="I5">
         <v>3480</v>
       </c>
-      <c r="D5">
-        <v>1920</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="J5">
+        <v>4320</v>
+      </c>
+      <c r="K5">
+        <v>5160</v>
+      </c>
+      <c r="L5">
+        <v>2640</v>
+      </c>
+      <c r="M5">
         <v>840</v>
       </c>
-      <c r="G5">
-        <v>1080</v>
-      </c>
-      <c r="H5">
-        <v>2160</v>
-      </c>
-      <c r="I5">
-        <v>1200</v>
-      </c>
-      <c r="J5">
-        <v>1680</v>
-      </c>
-      <c r="K5">
-        <v>2040</v>
-      </c>
-      <c r="L5">
-        <v>2880</v>
-      </c>
-      <c r="M5">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>3600</v>
+      </c>
+      <c r="O5">
+        <v>5760</v>
+      </c>
+      <c r="P5">
+        <v>3840</v>
+      </c>
+      <c r="Q5">
+        <v>720</v>
+      </c>
+      <c r="R5">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1509,40 +2180,55 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>3840</v>
+        <v>3960</v>
       </c>
       <c r="D6">
-        <v>2520</v>
+        <v>2400</v>
       </c>
       <c r="E6">
-        <v>840</v>
+        <v>2400</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>240</v>
+        <v>3600</v>
       </c>
       <c r="H6">
-        <v>1320</v>
+        <v>2160</v>
       </c>
       <c r="I6">
+        <v>4200</v>
+      </c>
+      <c r="J6">
+        <v>1920</v>
+      </c>
+      <c r="K6">
+        <v>2760</v>
+      </c>
+      <c r="L6">
+        <v>1440</v>
+      </c>
+      <c r="M6">
         <v>1560</v>
       </c>
-      <c r="J6">
-        <v>2280</v>
-      </c>
-      <c r="K6">
-        <v>1920</v>
-      </c>
-      <c r="L6">
-        <v>3720</v>
-      </c>
-      <c r="M6">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <v>4320</v>
+      </c>
+      <c r="O6">
+        <v>3360</v>
+      </c>
+      <c r="P6">
+        <v>2400</v>
+      </c>
+      <c r="Q6">
+        <v>3120</v>
+      </c>
+      <c r="R6">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1550,40 +2236,55 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>4080</v>
+        <v>1560</v>
       </c>
       <c r="D7">
-        <v>2760</v>
+        <v>3600</v>
       </c>
       <c r="E7">
-        <v>1080</v>
+        <v>2880</v>
       </c>
       <c r="F7">
-        <v>240</v>
+        <v>3600</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1080</v>
+        <v>1440</v>
       </c>
       <c r="I7">
         <v>1800</v>
       </c>
       <c r="J7">
-        <v>2520</v>
+        <v>4560</v>
       </c>
       <c r="K7">
-        <v>2160</v>
+        <v>2760</v>
       </c>
       <c r="L7">
-        <v>3960</v>
+        <v>5040</v>
       </c>
       <c r="M7">
-        <v>2040</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>2760</v>
+      </c>
+      <c r="N7">
+        <v>1200</v>
+      </c>
+      <c r="O7">
+        <v>3360</v>
+      </c>
+      <c r="P7">
+        <v>1440</v>
+      </c>
+      <c r="Q7">
+        <v>3120</v>
+      </c>
+      <c r="R7">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1591,40 +2292,55 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>3720</v>
+        <v>2280</v>
       </c>
       <c r="D8">
-        <v>3840</v>
+        <v>2160</v>
       </c>
       <c r="E8">
+        <v>1680</v>
+      </c>
+      <c r="F8">
         <v>2160</v>
       </c>
-      <c r="F8">
+      <c r="G8">
+        <v>1440</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>2040</v>
+      </c>
+      <c r="J8">
+        <v>3120</v>
+      </c>
+      <c r="K8">
+        <v>3480</v>
+      </c>
+      <c r="L8">
+        <v>3600</v>
+      </c>
+      <c r="M8">
         <v>1320</v>
       </c>
-      <c r="G8">
-        <v>1080</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
+      <c r="N8">
         <v>2160</v>
       </c>
-      <c r="J8">
-        <v>3600</v>
-      </c>
-      <c r="K8">
-        <v>1560</v>
-      </c>
-      <c r="L8">
-        <v>5040</v>
-      </c>
-      <c r="M8">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8">
+        <v>4080</v>
+      </c>
+      <c r="P8">
+        <v>2160</v>
+      </c>
+      <c r="Q8">
+        <v>2400</v>
+      </c>
+      <c r="R8">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1632,40 +2348,55 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>2280</v>
+        <v>3360</v>
       </c>
       <c r="D9">
-        <v>3120</v>
+        <v>4200</v>
       </c>
       <c r="E9">
-        <v>1200</v>
+        <v>3480</v>
       </c>
       <c r="F9">
-        <v>1560</v>
+        <v>4200</v>
       </c>
       <c r="G9">
         <v>1800</v>
       </c>
       <c r="H9">
-        <v>2160</v>
+        <v>2040</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>2880</v>
+        <v>5160</v>
       </c>
       <c r="K9">
-        <v>2040</v>
+        <v>4560</v>
       </c>
       <c r="L9">
-        <v>2880</v>
+        <v>5640</v>
       </c>
       <c r="M9">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>3360</v>
+      </c>
+      <c r="N9">
+        <v>600</v>
+      </c>
+      <c r="O9">
+        <v>5160</v>
+      </c>
+      <c r="P9">
+        <v>3240</v>
+      </c>
+      <c r="Q9">
+        <v>3240</v>
+      </c>
+      <c r="R9">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1673,40 +2404,55 @@
         <v>0</v>
       </c>
       <c r="C10">
+        <v>4920</v>
+      </c>
+      <c r="D10">
+        <v>4320</v>
+      </c>
+      <c r="E10">
+        <v>4320</v>
+      </c>
+      <c r="F10">
+        <v>1920</v>
+      </c>
+      <c r="G10">
+        <v>4560</v>
+      </c>
+      <c r="H10">
+        <v>3120</v>
+      </c>
+      <c r="I10">
         <v>5160</v>
       </c>
-      <c r="D10">
-        <v>240</v>
-      </c>
-      <c r="E10">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>3240</v>
+      </c>
+      <c r="L10">
         <v>1680</v>
       </c>
-      <c r="F10">
-        <v>2280</v>
-      </c>
-      <c r="G10">
-        <v>2520</v>
-      </c>
-      <c r="H10">
-        <v>3600</v>
-      </c>
-      <c r="I10">
-        <v>2880</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
+      <c r="M10">
         <v>3480</v>
       </c>
-      <c r="L10">
-        <v>4560</v>
-      </c>
-      <c r="M10">
-        <v>3120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>5280</v>
+      </c>
+      <c r="O10">
+        <v>1440</v>
+      </c>
+      <c r="P10">
+        <v>3360</v>
+      </c>
+      <c r="Q10">
+        <v>5040</v>
+      </c>
+      <c r="R10">
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1714,40 +2460,55 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>3600</v>
+        <v>1680</v>
       </c>
       <c r="D11">
+        <v>5160</v>
+      </c>
+      <c r="E11">
+        <v>5160</v>
+      </c>
+      <c r="F11">
+        <v>2760</v>
+      </c>
+      <c r="G11">
+        <v>2760</v>
+      </c>
+      <c r="H11">
+        <v>3480</v>
+      </c>
+      <c r="I11">
+        <v>4560</v>
+      </c>
+      <c r="J11">
+        <v>3240</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>3720</v>
       </c>
-      <c r="E11">
-        <v>2040</v>
-      </c>
-      <c r="F11">
-        <v>1920</v>
-      </c>
-      <c r="G11">
-        <v>2160</v>
-      </c>
-      <c r="H11">
-        <v>1560</v>
-      </c>
-      <c r="I11">
-        <v>2040</v>
-      </c>
-      <c r="J11">
-        <v>3480</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>4920</v>
-      </c>
       <c r="M11">
+        <v>4320</v>
+      </c>
+      <c r="N11">
+        <v>3960</v>
+      </c>
+      <c r="O11">
+        <v>1800</v>
+      </c>
+      <c r="P11">
         <v>1320</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="Q11">
+        <v>5880</v>
+      </c>
+      <c r="R11">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1755,40 +2516,55 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1320</v>
+        <v>5400</v>
       </c>
       <c r="D12">
-        <v>4800</v>
+        <v>2640</v>
       </c>
       <c r="E12">
-        <v>2880</v>
+        <v>2640</v>
       </c>
       <c r="F12">
+        <v>1440</v>
+      </c>
+      <c r="G12">
+        <v>5040</v>
+      </c>
+      <c r="H12">
+        <v>3600</v>
+      </c>
+      <c r="I12">
+        <v>5640</v>
+      </c>
+      <c r="J12">
+        <v>1680</v>
+      </c>
+      <c r="K12">
         <v>3720</v>
       </c>
-      <c r="G12">
-        <v>3960</v>
-      </c>
-      <c r="H12">
-        <v>5040</v>
-      </c>
-      <c r="I12">
-        <v>2880</v>
-      </c>
-      <c r="J12">
-        <v>4560</v>
-      </c>
-      <c r="K12">
-        <v>4920</v>
-      </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>2280</v>
+      </c>
+      <c r="N12">
+        <v>5760</v>
+      </c>
+      <c r="O12">
+        <v>3120</v>
+      </c>
+      <c r="P12">
+        <v>3840</v>
+      </c>
+      <c r="Q12">
+        <v>3360</v>
+      </c>
+      <c r="R12">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1796,36 +2572,331 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>3120</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1560</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2760</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1320</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>3360</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>3480</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>4320</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>2280</v>
       </c>
       <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>3480</v>
+      </c>
+      <c r="O13">
+        <v>4920</v>
+      </c>
+      <c r="P13">
+        <v>3000</v>
+      </c>
+      <c r="Q13">
+        <v>1560</v>
+      </c>
+      <c r="R13">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>2760</v>
+      </c>
+      <c r="D14">
+        <v>4320</v>
+      </c>
+      <c r="E14">
+        <v>3600</v>
+      </c>
+      <c r="F14">
+        <v>4320</v>
+      </c>
+      <c r="G14">
+        <v>1200</v>
+      </c>
+      <c r="H14">
+        <v>2160</v>
+      </c>
+      <c r="I14">
+        <v>600</v>
+      </c>
+      <c r="J14">
+        <v>5280</v>
+      </c>
+      <c r="K14">
+        <v>3960</v>
+      </c>
+      <c r="L14">
+        <v>5760</v>
+      </c>
+      <c r="M14">
+        <v>3480</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>4560</v>
+      </c>
+      <c r="P14">
+        <v>2640</v>
+      </c>
+      <c r="Q14">
+        <v>3360</v>
+      </c>
+      <c r="R14">
+        <v>4920</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>3480</v>
+      </c>
+      <c r="D15">
+        <v>5760</v>
+      </c>
+      <c r="E15">
+        <v>5760</v>
+      </c>
+      <c r="F15">
+        <v>3360</v>
+      </c>
+      <c r="G15">
+        <v>3360</v>
+      </c>
+      <c r="H15">
+        <v>4080</v>
+      </c>
+      <c r="I15">
+        <v>5160</v>
+      </c>
+      <c r="J15">
+        <v>1440</v>
+      </c>
+      <c r="K15">
+        <v>1800</v>
+      </c>
+      <c r="L15">
+        <v>3120</v>
+      </c>
+      <c r="M15">
+        <v>4920</v>
+      </c>
+      <c r="N15">
+        <v>4560</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1920</v>
+      </c>
+      <c r="Q15">
+        <v>6480</v>
+      </c>
+      <c r="R15">
+        <v>6120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1560</v>
+      </c>
+      <c r="D16">
+        <v>3840</v>
+      </c>
+      <c r="E16">
+        <v>3840</v>
+      </c>
+      <c r="F16">
+        <v>2400</v>
+      </c>
+      <c r="G16">
+        <v>1440</v>
+      </c>
+      <c r="H16">
+        <v>2160</v>
+      </c>
+      <c r="I16">
+        <v>3240</v>
+      </c>
+      <c r="J16">
+        <v>3360</v>
+      </c>
+      <c r="K16">
+        <v>1320</v>
+      </c>
+      <c r="L16">
+        <v>3840</v>
+      </c>
+      <c r="M16">
+        <v>3000</v>
+      </c>
+      <c r="N16">
+        <v>2640</v>
+      </c>
+      <c r="O16">
+        <v>1920</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>4560</v>
+      </c>
+      <c r="R16">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>4680</v>
+      </c>
+      <c r="D17">
+        <v>960</v>
+      </c>
+      <c r="E17">
+        <v>720</v>
+      </c>
+      <c r="F17">
+        <v>3120</v>
+      </c>
+      <c r="G17">
+        <v>3120</v>
+      </c>
+      <c r="H17">
+        <v>2400</v>
+      </c>
+      <c r="I17">
+        <v>3240</v>
+      </c>
+      <c r="J17">
+        <v>5040</v>
+      </c>
+      <c r="K17">
+        <v>5880</v>
+      </c>
+      <c r="L17">
+        <v>3360</v>
+      </c>
+      <c r="M17">
+        <v>1560</v>
+      </c>
+      <c r="N17">
+        <v>3360</v>
+      </c>
+      <c r="O17">
+        <v>6480</v>
+      </c>
+      <c r="P17">
+        <v>4560</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
         <v>0</v>
       </c>
     </row>

</xml_diff>